<commit_message>
-Updated files for experimento 1
</commit_message>
<xml_diff>
--- a/Resultados/Experimento1/Experimento1_[05_08_2023-20_35].xlsx
+++ b/Resultados/Experimento1/Experimento1_[05_08_2023-20_35].xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\denis\Desktop\Seminario\Codes\Datasets\MNIST_ORG\NN_Tests_DG\Resultados\Experimento1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B8343A3-E51E-4464-9294-F0D6CD107466}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3948D6B2-1FA9-4841-8544-0B6C529C7EBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -49,51 +49,7 @@
     <t>val_acc</t>
   </si>
   <si>
-    <t>[0, 0.9044733333333332, 0.9275933333333332, 0.9409333333333334, 0.9515866666666667, 0.9577666666666667, 0.9621266666666667, 0.9651200000000001, 0.96768, 0.96966, 0.9711266666666666, 0.9724066666666666, 0.9736066666666668, 0.9749733333333334, 0.9753666666666666, 0.9762066666666666, 0.9768133333333332, 0.9774066666666668, 0.9778533333333332, 0.9781533333333333, 0.9787933333333334, 0.9791866666666666, 0.9794999999999999, 0.9797933333333332, 0.9801200000000001, 0.98012, 0.98042, 0.9806666666666666, 0.9809933333333334, 0.9810866666666668, 0.9815066666666666, 0.9815733333333334, 0.9817666666666666, 0.9819533333333332, 0.9820666666666666, 0.9819733333333333, 0.9820999999999999, 0.9823066666666668, 0.9823666666666667, 0.9823666666666665, 0.9825733333333333, 0.9827266666666665, 0.9827066666666667, 0.9827400000000001, 0.9830866666666666, 0.9832466666666666, 0.9831799999999998, 0.9831666666666664, 0.9830266666666668, 0.9832199999999999, 0.9833066666666668, 0.98334, 0.9831666666666667, 0.9834133333333333, 0.9834, 0.9834933333333333, 0.9836066666666666, 0.9835, 0.9837400000000002, 0.9837266666666667, 0.9836866666666668, 0.9838399999999999, 0.9838266666666666, 0.9837533333333336, 0.98364, 0.9837266666666665, 0.9836933333333334, 0.9837399999999998, 0.98378, 0.9839933333333335, 0.9839466666666667, 0.98424, 0.9841266666666666, 0.9839933333333334, 0.9841200000000001, 0.9841133333333334, 0.9840400000000001, 0.9842400000000001, 0.9841933333333335, 0.9841333333333334, 0.9841666666666667, 0.9840933333333335, 0.9841333333333335, 0.9842999999999998, 0.9844, 0.9843866666666666, 0.9842466666666669, 0.9842866666666665, 0.9843933333333332, 0.9841133333333334, 0.9842733333333334, 0.9843466666666667, 0.9843200000000001, 0.9844600000000001, 0.9843933333333333, 0.9845733333333332, 0.9842733333333332, 0.9844200000000001, 0.9844399999999999, 0.9846466666666666, 0.9845600000000002]</t>
-  </si>
-  <si>
-    <t>98.39%</t>
-  </si>
-  <si>
-    <t>[0.4237412949403127, 0.313975128531456, 0.26324957609176636, 0.20376050770282744, 0.1779392754038175, 0.1753847450017929, 0.15560612926880518, 0.1425825575987498, 0.11470940609773, 0.11560600996017456, 0.10549678256114324, 0.10697309921185176, 0.08941234027345975, 0.08392823760708173, 0.08337226584553718, 0.07583315086861452, 0.06524490416049958, 0.06564390162626903, 0.06666812772552172, 0.0637959656616052, 0.07516517067948977, 0.05988484223683675, 0.05540787701805432, 0.052514573683341344, 0.055692929898699124, 0.04819255601614714, 0.04756878229478995, 0.039933432390292484, 0.0373108779390653, 0.04195826885600885, 0.04322190545499325, 0.03204781077802181, 0.03490916322916746, 0.032441829517483714, 0.035255984279016654, 0.032766964038213095, 0.0300863994906346, 0.026628659230967362, 0.027494045409063497, 0.03218472171574831, 0.02538345642387867, 0.02717021300146977, 0.021856550375620523, 0.019784910542269548, 0.021598451895018418, 0.025528955832123758, 0.020893959514796733, 0.019803445041179656, 0.017660305617998043, 0.020575175651659568, 0.016336557827889918, 0.01623681594307224, 0.01875797895093759, 0.020151794515550138, 0.015968418680131435, 0.016670621590067942, 0.012343587819486856, 0.017305121819178263, 0.016284191670517128, 0.011843906156718731, 0.013183899596333504, 0.013353999238461256, 0.013466999121010303, 0.010611642369379599, 0.014599335752427578, 0.009991950091595451, 0.011540451475108663, 0.01264147162437439, 0.010239168691138426, 0.011854765564203262, 0.009990526021768649, 0.007818627295394738, 0.008865329157561063, 0.008707391222318013, 0.00917873348419865, 0.008776655529315273, 0.009880615305155516, 0.009418641154964765, 0.010504577246805032, 0.007686068847154577, 0.007874760388707122, 0.009548894874751569, 0.00927191066245238, 0.007783232877651851, 0.008582017881174882, 0.008814505239327749, 0.007996547734364867, 0.006697049473101894, 0.009336886911963422, 0.006552621551478902, 0.006868223287165165, 0.0061003280648340786, 0.005143942210512857, 0.008406765246763825, 0.006560344792281588, 0.006333055316160122, 0.006073501488814751, 0.005296442890539765, 0.0055449812284981215, 0.007864593078071873]</t>
-  </si>
-  <si>
-    <t>[[9.71333333e+02 4.00000000e-01 8.66666667e-01 8.00000000e-01
-  4.00000000e-01 5.33333333e-01 2.40000000e+00 1.06666667e+00
-  1.80000000e+00 4.00000000e-01]
- [0.00000000e+00 1.12700000e+03 2.13333333e+00 5.33333333e-01
-  0.00000000e+00 8.00000000e-01 1.80000000e+00 8.00000000e-01
-  1.93333333e+00 0.00000000e+00]
- [2.73333333e+00 1.26666667e+00 1.01546667e+03 1.33333333e+00
-  1.40000000e+00 0.00000000e+00 1.46666667e+00 5.53333333e+00
-  2.80000000e+00 0.00000000e+00]
- [1.33333333e-01 0.00000000e+00 2.93333333e+00 9.93800000e+02
-  0.00000000e+00 4.00000000e+00 0.00000000e+00 3.26666667e+00
-  3.40000000e+00 2.46666667e+00]
- [1.00000000e+00 0.00000000e+00 1.80000000e+00 6.66666667e-01
-  9.64866667e+02 0.00000000e+00 3.60000000e+00 1.53333333e+00
-  2.66666667e-01 8.26666667e+00]
- [2.46666667e+00 0.00000000e+00 0.00000000e+00 6.26666667e+00
-  9.33333333e-01 8.73533333e+02 4.40000000e+00 7.33333333e-01
-  2.26666667e+00 1.40000000e+00]
- [3.06666667e+00 2.26666667e+00 4.00000000e-01 9.33333333e-01
-  2.73333333e+00 3.33333333e+00 9.44800000e+02 0.00000000e+00
-  4.66666667e-01 0.00000000e+00]
- [1.00000000e+00 3.86666667e+00 7.53333333e+00 1.60000000e+00
-  2.00000000e-01 0.00000000e+00 0.00000000e+00 1.00786667e+03
-  2.06666667e+00 3.86666667e+00]
- [2.13333333e+00 0.00000000e+00 1.86666667e+00 3.06666667e+00
-  2.60000000e+00 2.00000000e+00 1.46666667e+00 3.93333333e+00
-  9.54066667e+02 2.86666667e+00]
- [2.73333333e+00 2.13333333e+00 0.00000000e+00 3.53333333e+00
-  6.86666667e+00 1.86666667e+00 8.00000000e-01 4.26666667e+00
-  6.66666667e-01 9.86133333e+02]]</t>
-  </si>
-  <si>
     <t>[0.0, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01]</t>
-  </si>
-  <si>
-    <t>98.46%</t>
   </si>
   <si>
     <t>[0, 0.9052066666666667, 0.9280733333333334, 0.9418066666666666, 0.9515933333333333, 0.9577666666666665, 0.9624, 0.9653133333333331, 0.9677333333333333, 0.9699533333333334, 0.9713933333333332, 0.9722799999999999, 0.9736533333333333, 0.9743266666666665, 0.9754266666666668, 0.97606, 0.9767933333333333, 0.9775133333333332, 0.9777666666666666, 0.9780866666666667, 0.9785400000000001, 0.9790533333333331, 0.9795200000000001, 0.9798133333333333, 0.9800133333333334, 0.9803066666666668, 0.9805133333333333, 0.9806199999999999, 0.9809866666666666, 0.9811000000000001, 0.9812933333333332, 0.9814200000000001, 0.9817266666666669, 0.9819066666666668, 0.9816666666666667, 0.9821666666666665, 0.9823266666666667, 0.98232, 0.9825333333333333, 0.98256, 0.9825533333333335, 0.98252, 0.9827999999999999, 0.9828466666666666, 0.98312, 0.9829266666666666, 0.9831133333333335, 0.9830000000000001, 0.9830333333333333, 0.9833000000000001, 0.9831800000000002, 0.9832733333333334, 0.9834066666666668, 0.9834799999999999, 0.9833666666666667, 0.9833866666666666, 0.9834666666666667, 0.9837866666666666, 0.9837333333333332, 0.9835999999999999, 0.9838266666666666, 0.9838533333333334, 0.9837400000000002, 0.9837666666666666, 0.9837933333333334, 0.9839066666666665, 0.98378, 0.9840266666666667, 0.9840466666666668, 0.9838333333333334, 0.9840666666666666, 0.9840266666666667, 0.9841266666666666, 0.9839799999999997, 0.9840600000000002, 0.9839333333333332, 0.9840466666666667, 0.9839866666666667, 0.9840999999999999, 0.9839866666666667, 0.9840266666666668, 0.9841199999999998, 0.9840199999999998, 0.98408, 0.9842666666666667, 0.9841000000000001, 0.9840066666666666, 0.9841266666666667, 0.9842866666666665, 0.9841866666666668, 0.9843199999999999, 0.9842066666666667, 0.9842933333333332, 0.9842066666666666, 0.9844266666666667, 0.9841266666666667, 0.9844000000000002, 0.9841066666666667, 0.9843533333333333, 0.9843933333333331, 0.9844533333333334]</t>
@@ -237,51 +193,10 @@
     <t>[0.0, 0.0822601719926907, 0.08272603676931584, 0.08657725941663964, 0.09021303967261031, 0.06104829237147001, 0.026130336616707377, 0.022441102255778226, 0.016598446986262862, 0.09968865226057674, 0.09982633773045364, 0.09989334504074544, 0.10000562287379025, 0.0606198861383859, 0.014683137475080009, 0.013820155782280408, 0.013170059842204172, 0.07906065218457764, 0.08627142690710798, 0.09866458170130239, 0.10058973892004247, 0.08052460254759153, 0.06204243871923165, 0.010158919096318685, 0.010069189373219212, 0.03210634267000377, 0.04400134669178596, 0.0543436761134716, 0.09035261366842527, 0.04765171735458618, 0.016358445493554245, 0.010298972273427026, 0.00911335395213533, 0.07363675099254556, 0.09022064683625433, 0.09239781151115213, 0.09843588286552683, 0.027636266973611406, 0.0233815959762819, 0.019435309800166653, 0.013249267870538574, 0.05598691608098044, 0.09245522663838429, 0.09698790289608782, 0.09908960625852767, 0.09004629758515502, 0.07639912571442971, 0.05900403655526589, 0.035545441892925286, 0.052968965375715826, 0.08887166481362896, 0.09562276063372273, 0.09961585060226143, 0.030463733243401396, 0.029367166290413006, 0.021654601128862954, 0.01488968317981327, 0.08567144761179249, 0.09422604455242525, 0.09952188739829279, 0.09969825882335452, 0.02610183037604215, 0.024110865914313842, 0.020050117836887565, 0.00953637657246732, 0.04149001695642171, 0.05550168953188844, 0.08114808046298976, 0.09477719742714946, 0.02667449946574628, 0.012255052925040118, 0.011267094375013914, 0.010484123692447106, 0.069269949020049, 0.09913858113615157, 0.09989748507324074, 0.10033175058270218, 0.0453848370204304, 0.032373495119098636, 0.03079321625790868, 0.020672167949786067, 0.09859613680221407, 0.09865567240066798, 0.09927784539257675, 0.09960827996311085, 0.08189627715852398, 0.01804575109823532, 0.012858829014844805, 0.010695562696472313, 0.03678119637098212, 0.053707792281114886, 0.061252040758634205, 0.08438816601885418, 0.0262844802734769, 0.014494084895260485, 0.011068787466299811, 0.009338979483128684, 0.018212591272605612, 0.048708451828542096, 0.0824119362040578, 0.08737177704206403]</t>
   </si>
   <si>
-    <t>[0, 0.92244, 0.9712200000000001, 0.9783866666666666, 0.9807000000000001, 0.9804733333333331, 0.9804399999999999, 0.9804399999999999, 0.9804399999999999, 0.9804399999999999, 0.9804399999999999, 0.9804399999999999, 0.9804399999999999, 0.9804399999999999, 0.9804399999999999, 0.9804399999999999, 0.9804399999999999, 0.9804399999999999, 0.9804399999999999, 0.9804399999999999, 0.9804399999999999, 0.9804399999999999, 0.9804399999999999, 0.9804399999999999, 0.9804399999999999, 0.9804399999999999, 0.9804399999999999, 0.9804399999999999, 0.9804399999999999, 0.9804399999999999, 0.9804399999999999, 0.9804399999999999, 0.9804399999999999, 0.9804399999999999, 0.9804399999999999, 0.9804399999999999, 0.9804399999999999, 0.9804399999999999, 0.9804399999999999, 0.9804399999999999, 0.9804399999999999, 0.9804399999999999, 0.9804399999999999, 0.9804399999999999, 0.9804399999999999, 0.9804399999999999, 0.9804399999999999, 0.9804399999999999, 0.9804399999999999, 0.9804399999999999, 0.9804399999999999, 0.9804399999999999, 0.9804399999999999, 0.9804399999999999, 0.9804399999999999, 0.9804399999999999, 0.9804399999999999, 0.9804399999999999, 0.9804399999999999, 0.9804399999999999, 0.9804399999999999, 0.9804399999999999, 0.9804399999999999, 0.9804399999999999, 0.9804399999999999, 0.9804399999999999, 0.9804399999999999, 0.9804399999999999, 0.9804399999999999, 0.9804399999999999, 0.9804399999999999, 0.9804399999999999, 0.9804399999999999, 0.9804399999999999, 0.9804399999999999, 0.9804399999999999, 0.9804399999999999, 0.9804399999999999, 0.9804399999999999, 0.9804399999999999, 0.9804399999999999, 0.9804399999999999, 0.9804399999999999, 0.9804399999999999, 0.9804399999999999, 0.9804399999999999, 0.9804399999999999, 0.9804399999999999, 0.9804399999999999, 0.9804399999999999, 0.9804399999999999, 0.9804399999999999, 0.9804399999999999, 0.9804399999999999, 0.9804399999999999, 0.9804399999999999, 0.9804399999999999, 0.9804399999999999, 0.9804399999999999, 0.9804399999999999, 0.9804399999999999]</t>
-  </si>
-  <si>
     <t>98.07%</t>
   </si>
   <si>
-    <t>[2.3080369313557942, 0.2787556638320287, 0.0761029876768589, 0.014674305853744348, 0.0003744480719130176, 9.920426649046021e-07, 1.1939229883258424e-07, 1.1939229883258424e-07, 1.1939229883258424e-07, 1.1939229883258424e-07, 1.1939229883258424e-07, 1.1939229883258424e-07, 1.1939229883258424e-07, 1.1939229883258424e-07, 1.1939229883258424e-07, 1.1939229883258424e-07, 1.1939229883258424e-07, 1.1939229883258424e-07, 1.1939229883258424e-07, 1.1939229883258424e-07, 1.1939229883258424e-07, 1.1939229883258424e-07, 1.1939229883258424e-07, 1.1939229883258424e-07, 1.1939229883258424e-07, 1.1939229883258424e-07, 1.1939229883258424e-07, 1.1939229883258424e-07, 1.1939229883258424e-07, 1.1939229883258424e-07, 1.1939229883258424e-07, 1.1939229883258424e-07, 1.1939229883258424e-07, 1.1939229883258424e-07, 1.1939229883258424e-07, 1.1939229883258424e-07, 1.1939229883258424e-07, 1.1939229883258424e-07, 1.1939229883258424e-07, 1.1939229883258424e-07, 1.1939229883258424e-07, 1.1939229883258424e-07, 1.1939229883258424e-07, 1.1939229883258424e-07, 1.1939229883258424e-07, 1.1939229883258424e-07, 1.1939229883258424e-07, 1.1939229883258424e-07, 1.1939229883258424e-07, 1.1939229883258424e-07, 1.1939229883258424e-07, 1.1939229883258424e-07, 1.1939229883258424e-07, 1.1939229883258424e-07, 1.1939229883258424e-07, 1.1939229883258424e-07, 1.1939229883258424e-07, 1.1939229883258424e-07, 1.1939229883258424e-07, 1.1939229883258424e-07, 1.1939229883258424e-07, 1.1939229883258424e-07, 1.1939229883258424e-07, 1.1939229883258424e-07, 1.1939229883258424e-07, 1.1939229883258424e-07, 1.1939229883258424e-07, 1.1939229883258424e-07, 1.1939229883258424e-07, 1.1939229883258424e-07, 1.1939229883258424e-07, 1.1939229883258424e-07, 1.1939229883258424e-07, 1.1939229883258424e-07, 1.1939229883258424e-07, 1.1939229883258424e-07, 1.1939229883258424e-07, 1.1939229883258424e-07, 1.1939229883258424e-07, 1.1939229883258424e-07, 1.1939229883258424e-07, 1.1939229883258424e-07, 1.1939229883258424e-07, 1.1939229883258424e-07, 1.1939229883258424e-07, 1.1939229883258424e-07, 1.1939229883258424e-07, 1.1939229883258424e-07, 1.1939229883258424e-07, 1.1939229883258424e-07, 1.1939229883258424e-07, 1.1939229883258424e-07, 1.1939229883258424e-07, 1.1939229883258424e-07, 1.1939229883258424e-07, 1.1939229883258424e-07, 1.1939229883258424e-07, 1.1939229883258424e-07, 1.1939229883258424e-07, 1.1939229883258424e-07]</t>
-  </si>
-  <si>
-    <t>[[9.69800000e+02 3.33333333e-01 2.66666667e+00 6.66666667e-02
-  4.66666667e-01 1.13333333e+00 2.26666667e+00 1.00000000e+00
-  1.73333333e+00 5.33333333e-01]
- [3.33333333e-01 1.12746667e+03 1.80000000e+00 5.33333333e-01
-  0.00000000e+00 9.33333333e-01 1.13333333e+00 8.66666667e-01
-  1.80000000e+00 1.33333333e-01]
- [2.46666667e+00 1.33333333e+00 1.00986667e+03 4.20000000e+00
-  1.73333333e+00 0.00000000e+00 1.60000000e+00 5.93333333e+00
-  4.73333333e+00 1.33333333e-01]
- [9.33333333e-01 2.66666667e-01 4.00000000e+00 9.90533333e+02
-  0.00000000e+00 4.40000000e+00 0.00000000e+00 2.20000000e+00
-  4.73333333e+00 2.93333333e+00]
- [1.06666667e+00 4.00000000e-01 2.00000000e+00 9.33333333e-01
-  9.60666667e+02 4.66666667e-01 3.40000000e+00 1.80000000e+00
-  3.33333333e-01 1.09333333e+01]
- [1.93333333e+00 6.66666667e-02 0.00000000e+00 9.20000000e+00
-  7.33333333e-01 8.68200000e+02 4.20000000e+00 7.33333333e-01
-  2.60000000e+00 4.33333333e+00]
- [3.80000000e+00 2.26666667e+00 1.06666667e+00 9.33333333e-01
-  4.26666667e+00 2.73333333e+00 9.40800000e+02 2.00000000e-01
-  1.93333333e+00 0.00000000e+00]
- [6.00000000e-01 2.66666667e+00 6.60000000e+00 2.33333333e+00
-  1.46666667e+00 0.00000000e+00 0.00000000e+00 1.00700000e+03
-  2.53333333e+00 4.80000000e+00]
- [2.20000000e+00 6.66666667e-02 2.33333333e+00 5.80000000e+00
-  1.00000000e+00 2.60000000e+00 2.46666667e+00 2.93333333e+00
-  9.50533333e+02 4.06666667e+00]
- [2.00000000e+00 2.33333333e+00 4.66666667e-01 3.46666667e+00
-  8.26666667e+00 3.13333333e+00 1.46666667e+00 4.46666667e+00
-  1.73333333e+00 9.81666667e+02]]</t>
-  </si>
-  <si>
     <t>[0]</t>
-  </si>
-  <si>
-    <t>98.04%</t>
   </si>
   <si>
     <t>[0, 0.10030666666666667, 0.6526933333333333, 0.5812933333333332, 0.70922, 0.7796133333333335, 0.8093866666666668, 0.8275, 0.8355266666666666, 0.8428666666666665, 0.8571066666666667, 0.8603466666666666, 0.8707933333333333, 0.8752866666666665, 0.88294, 0.8872066666666665, 0.8919933333333334, 0.8966999999999998, 0.8985133333333334, 0.9036000000000001, 0.9065933333333334, 0.9105666666666664, 0.9130533333333335, 0.91676, 0.91934, 0.9216933333333333, 0.9247666666666667, 0.9277066666666667, 0.9306, 0.93262, 0.9348466666666665, 0.9372466666666667, 0.9397733333333333, 0.9425733333333335, 0.9444333333333332, 0.9458266666666667, 0.9479466666666666, 0.9490533333333333, 0.9506600000000002, 0.9516933333333333, 0.95362, 0.9541666666666667, 0.9560666666666666, 0.9573266666666667, 0.9581799999999999, 0.9595, 0.96022, 0.9613933333333334, 0.9625, 0.96346, 0.9642933333333333, 0.9648733333333331, 0.9660133333333333, 0.9663799999999999, 0.9668733333333334, 0.9677600000000001, 0.9685333333333331, 0.96874, 0.9695466666666667, 0.9701466666666665, 0.9703400000000001, 0.9707533333333332, 0.9719266666666665, 0.9721866666666668, 0.9725000000000001, 0.9727999999999998, 0.9735066666666666, 0.9738933333333334, 0.974, 0.9744066666666666, 0.9741866666666668, 0.9745066666666666, 0.9744333333333333, 0.9749133333333333, 0.9755199999999998, 0.9756866666666667, 0.9760933333333334, 0.9757333333333332, 0.9758733333333333, 0.9765933333333333, 0.9768933333333332, 0.9772466666666666, 0.9772866666666666, 0.9775866666666667, 0.9778800000000001, 0.9775133333333333, 0.9778333333333332, 0.9780133333333334, 0.9780266666666666, 0.9782333333333334, 0.9784733333333333, 0.9786133333333334, 0.9786266666666666, 0.97892, 0.9789466666666667, 0.9791133333333331, 0.9793133333333335, 0.97918, 0.9792866666666667, 0.97954, 0.9794266666666668]</t>
@@ -513,9 +428,6 @@
     <t>TA Ciclica</t>
   </si>
   <si>
-    <t>L-BFGS con BL</t>
-  </si>
-  <si>
     <t>L-BFGS</t>
   </si>
   <si>
@@ -526,6 +438,94 @@
   </si>
   <si>
     <t>TA Ciclica Aleatoria Extendida</t>
+  </si>
+  <si>
+    <t>[[9.59533333e+02 1.00000000e+00 3.33333333e-01 6.66666667e-02
+  3.33333333e-01 1.33333333e-01 3.00000000e+00 1.20000000e+00
+  1.10666667e+01 3.33333333e+00]
+ [6.66666667e-02 1.11786667e+03 1.93333333e+00 1.60000000e+00
+  8.00000000e-01 1.86666667e+00 1.33333333e+00 1.33333333e-01
+  7.13333333e+00 2.26666667e+00]
+ [1.46666667e+00 1.26666667e+00 9.94933333e+02 1.73333333e+00
+  6.66666667e-01 6.66666667e-02 1.33333333e+00 5.86666667e+00
+  1.92666667e+01 5.40000000e+00]
+ [6.66666667e-02 2.00000000e-01 6.13333333e+00 9.56066667e+02
+  0.00000000e+00 7.06666667e+00 0.00000000e+00 3.40000000e+00
+  2.61333333e+01 1.09333333e+01]
+ [2.66666667e-01 5.33333333e-01 1.40000000e+00 0.00000000e+00
+  9.34533333e+02 6.66666667e-02 4.46666667e+00 8.66666667e-01
+  1.64666667e+01 2.34000000e+01]
+ [1.60000000e+00 6.00000000e-01 5.33333333e-01 8.26666667e+00
+  5.33333333e-01 8.42133333e+02 5.00000000e+00 6.00000000e-01
+  2.38000000e+01 8.93333333e+00]
+ [3.06666667e+00 2.73333333e+00 6.00000000e-01 0.00000000e+00
+  4.60000000e+00 6.66666667e+00 9.16666667e+02 0.00000000e+00
+  2.00000000e+01 3.66666667e+00]
+ [3.33333333e-01 2.06666667e+00 1.12666667e+01 2.66666667e+00
+  5.33333333e-01 6.66666667e-02 0.00000000e+00 9.80400000e+02
+  1.76000000e+01 1.30666667e+01]
+ [1.06666667e+00 6.00000000e-01 2.06666667e+00 1.20000000e+00
+  3.26666667e+00 3.06666667e+00 6.66666667e-01 2.20000000e+00
+  9.42266667e+02 1.76000000e+01]
+ [1.00000000e+00 2.53333333e+00 8.00000000e-01 3.20000000e+00
+  7.26666667e+00 1.46666667e+00 6.66666667e-02 2.93333333e+00
+  3.28666667e+01 9.56866667e+02]]</t>
+  </si>
+  <si>
+    <t>[0.5544816573460897, 0.32983689109484354, 0.3014120012521744, 0.25957137246926626, 0.2690966367721558, 0.2712463438510895, 0.2703043142954508, 0.24017351468404133, 0.23537714580694835, 0.2502383400996526, 0.23073100944360098, 0.23464338580767313, 0.19570245494445165, 0.2169069061676661, 0.2179017166296641, 0.2413592557112376, 0.23434856583674749, 0.23284405420223872, 0.20887525379657745, 0.27176660945018133, 0.20709295123815535, 0.21583271225293477, 0.24097758829593657, 0.16883669992287953, 0.253985961774985, 0.24540594816207886, 0.18797782783706982, 0.18714656680822372, 0.23281653076410294, 0.2336189220348994, 0.22195943892002107, 0.23588998019695281, 0.20033715069293975, 0.23038256516059238, 0.22108551611502966, 0.2326188713312149, 0.23811996579170228, 0.2635813082257907, 0.24287398060162863, 0.21393826305866243, 0.21200314511855442, 0.23157978554566702, 0.21054855684439341, 0.24400915851195654, 0.2373494029045105, 0.23284271011749905, 0.22346876015265782, 0.30882172683874765, 0.27738828311363856, 0.23123506953318915, 0.21512128114700318, 0.2062379851937294, 0.2465719997882843, 0.28929530481497445, 0.26980694830417634, 0.28728978087504703, 0.2709815646211306, 0.2298703948656718, 0.3045196304718653, 0.25642593403657277, 0.25522035857041675, 0.2745922029018402, 0.3206243475278219, 0.23300176163514455, 0.3514337296287219, 0.30233253836631774, 0.18874629686276118, 0.2715308427810669, 0.28709758073091507, 0.25366740028063456, 0.30904223918914797, 0.3047352209687233, 0.21695175170898437, 0.22519503235816957, 0.38196333895126977, 0.4189537356297175, 0.5303281615177791, 0.30176957994699477, 0.3448551997542381, 0.25163766493399936, 0.26136313180128734, 0.23949182977279027, 0.27569872935613, 0.4394766132036845, 0.3470660110314687, 0.35644853810469307, 0.30032102366288504, 0.2975920076171557, 0.27947490811347964, 0.30396843552589414, 0.3093000580867132, 0.3030782530705134, 0.3497876634200414, 0.353869891166687, 0.2350054870049159, 0.30730666071176527, 0.2765252023935318, 0.2577137231826782, 0.26162790060043334, 0.32860462963581083]</t>
+  </si>
+  <si>
+    <t>[0, 0.8908533333333334, 0.9340933333333332, 0.9480266666666668, 0.9497800000000001, 0.9578599999999999, 0.9562933333333332, 0.95834, 0.96004, 0.9598800000000001, 0.9604266666666668, 0.9645066666666665, 0.96538, 0.9653133333333334, 0.9659733333333335, 0.9673933333333333, 0.9682866666666665, 0.9656533333333333, 0.9664999999999999, 0.9684133333333332, 0.9660799999999998, 0.9687533333333335, 0.9670866666666667, 0.96914, 0.9704333333333335, 0.9666733333333332, 0.9685600000000001, 0.9714200000000002, 0.9693733333333333, 0.9670799999999999, 0.9704400000000001, 0.9709133333333335, 0.9695466666666666, 0.9694400000000001, 0.9696933333333334, 0.9691066666666668, 0.9703133333333334, 0.9690333333333333, 0.9694933333333334, 0.9695800000000001, 0.9705733333333332, 0.96888, 0.9692266666666668, 0.9698666666666665, 0.9696999999999999, 0.9687933333333335, 0.9694866666666668, 0.9684533333333333, 0.9693933333333333, 0.96778, 0.9689666666666668, 0.9668666666666668, 0.9698000000000001, 0.9696733333333333, 0.9679333333333334, 0.9701066666666667, 0.96822, 0.9678733333333335, 0.9678799999999999, 0.9696, 0.9678599999999998, 0.9660933333333334, 0.9676799999999999, 0.9669399999999999, 0.9672666666666667, 0.9675466666666668, 0.9681666666666666, 0.9680400000000001, 0.96662, 0.9657199999999999, 0.9664866666666667, 0.9675133333333332, 0.9654266666666668, 0.9677533333333332, 0.9683000000000003, 0.9655933333333332, 0.9663666666666668, 0.9660666666666667, 0.9659133333333332, 0.9656999999999999, 0.9673533333333332, 0.9659866666666667, 0.9674200000000001, 0.9661533333333333, 0.9646533333333333, 0.9630866666666669, 0.9650666666666666, 0.9666133333333332, 0.9656533333333335, 0.9653266666666666, 0.9632600000000001, 0.9644733333333334, 0.9624799999999999, 0.9621133333333333, 0.9626866666666667, 0.9639800000000001, 0.9642866666666665, 0.9617599999999998, 0.9641733333333333, 0.9623133333333332, 0.9640533333333334]</t>
+  </si>
+  <si>
+    <t>96.01%</t>
+  </si>
+  <si>
+    <t>96.41%</t>
+  </si>
+  <si>
+    <t>[0, 0.8679933333333333, 0.9660133333333333, 0.9766666666666668, 0.9797733333333333, 0.9804733333333334, 0.9806866666666667, 0.9807666666666667, 0.9808, 0.98078, 0.98078, 0.98078, 0.98078, 0.98078, 0.98078, 0.98078, 0.98078, 0.98078, 0.98078, 0.98078, 0.98078, 0.98078, 0.98078, 0.98078, 0.98078, 0.98078, 0.98078, 0.98078, 0.98078, 0.98078, 0.98078, 0.98078, 0.98078, 0.98078, 0.98078, 0.98078, 0.98078, 0.98078, 0.98078, 0.98078, 0.98078, 0.98078, 0.98078, 0.98078, 0.98078, 0.98078, 0.98078, 0.98078, 0.98078, 0.98078, 0.98078, 0.98078, 0.98078, 0.98078, 0.98078, 0.98078, 0.98078, 0.98078, 0.98078, 0.98078, 0.98078, 0.98078, 0.98078, 0.98078, 0.98078, 0.98078, 0.98078, 0.98078, 0.98078, 0.98078, 0.98078, 0.98078, 0.98078, 0.98078, 0.98078, 0.98078, 0.98078, 0.98078, 0.98078, 0.98078, 0.98078, 0.98078, 0.98078, 0.98078, 0.98078, 0.98078, 0.98078, 0.98078, 0.98078, 0.98078, 0.98078, 0.98078, 0.98078, 0.98078, 0.98078, 0.98078, 0.98078, 0.98078, 0.98078, 0.98078, 0.98078]</t>
+  </si>
+  <si>
+    <t>[2.305495516459147, 0.4199754198392232, 0.0972831462820371, 0.027571307557324568, 0.006602380151161924, 0.0027555351184105348, 0.0008286219513081505, 7.88416437842443e-05, 1.7773248089270055e-06, 9.053088424100983e-08, 9.053088424100983e-08, 9.053088424100983e-08, 9.053088424100983e-08, 9.053088424100983e-08, 9.053088424100983e-08, 9.053088424100983e-08, 9.053088424100983e-08, 9.053088424100983e-08, 9.053088424100983e-08, 9.053088424100983e-08, 9.053088424100983e-08, 9.053088424100983e-08, 9.053088424100983e-08, 9.053088424100983e-08, 9.053088424100983e-08, 9.053088424100983e-08, 9.053088424100983e-08, 9.053088424100983e-08, 9.053088424100983e-08, 9.053088424100983e-08, 9.053088424100983e-08, 9.053088424100983e-08, 9.053088424100983e-08, 9.053088424100983e-08, 9.053088424100983e-08, 9.053088424100983e-08, 9.053088424100983e-08, 9.053088424100983e-08, 9.053088424100983e-08, 9.053088424100983e-08, 9.053088424100983e-08, 9.053088424100983e-08, 9.053088424100983e-08, 9.053088424100983e-08, 9.053088424100983e-08, 9.053088424100983e-08, 9.053088424100983e-08, 9.053088424100983e-08, 9.053088424100983e-08, 9.053088424100983e-08, 9.053088424100983e-08, 9.053088424100983e-08, 9.053088424100983e-08, 9.053088424100983e-08, 9.053088424100983e-08, 9.053088424100983e-08, 9.053088424100983e-08, 9.053088424100983e-08, 9.053088424100983e-08, 9.053088424100983e-08, 9.053088424100983e-08, 9.053088424100983e-08, 9.053088424100983e-08, 9.053088424100983e-08, 9.053088424100983e-08, 9.053088424100983e-08, 9.053088424100983e-08, 9.053088424100983e-08, 9.053088424100983e-08, 9.053088424100983e-08, 9.053088424100983e-08, 9.053088424100983e-08, 9.053088424100983e-08, 9.053088424100983e-08, 9.053088424100983e-08, 9.053088424100983e-08, 9.053088424100983e-08, 9.053088424100983e-08, 9.053088424100983e-08, 9.053088424100983e-08, 9.053088424100983e-08, 9.053088424100983e-08, 9.053088424100983e-08, 9.053088424100983e-08, 9.053088424100983e-08, 9.053088424100983e-08, 9.053088424100983e-08, 9.053088424100983e-08, 9.053088424100983e-08, 9.053088424100983e-08, 9.053088424100983e-08, 9.053088424100983e-08, 9.053088424100983e-08, 9.053088424100983e-08, 9.053088424100983e-08, 9.053088424100983e-08, 9.053088424100983e-08, 9.053088424100983e-08, 9.053088424100983e-08, 9.053088424100983e-08]</t>
+  </si>
+  <si>
+    <t>[[9.69733333e+02 4.00000000e-01 2.13333333e+00 6.66666667e-02
+  5.33333333e-01 1.13333333e+00 2.06666667e+00 8.00000000e-01
+  2.00000000e+00 1.13333333e+00]
+ [1.33333333e-01 1.12760000e+03 1.53333333e+00 5.33333333e-01
+  0.00000000e+00 1.06666667e+00 1.26666667e+00 6.00000000e-01
+  2.06666667e+00 2.00000000e-01]
+ [2.46666667e+00 1.06666667e+00 1.00940000e+03 4.60000000e+00
+  1.73333333e+00 0.00000000e+00 1.93333333e+00 5.60000000e+00
+  5.06666667e+00 1.33333333e-01]
+ [7.33333333e-01 2.66666667e-01 3.26666667e+00 9.91933333e+02
+  0.00000000e+00 4.26666667e+00 0.00000000e+00 2.26666667e+00
+  5.20000000e+00 2.06666667e+00]
+ [8.00000000e-01 1.33333333e-01 2.33333333e+00 6.00000000e-01
+  9.59733333e+02 3.33333333e-01 3.86666667e+00 1.26666667e+00
+  8.00000000e-01 1.21333333e+01]
+ [2.06666667e+00 6.66666667e-02 1.33333333e-01 1.12666667e+01
+  8.00000000e-01 8.65800000e+02 4.46666667e+00 6.00000000e-01
+  2.73333333e+00 4.06666667e+00]
+ [3.60000000e+00 2.53333333e+00 9.33333333e-01 7.33333333e-01
+  4.06666667e+00 2.80000000e+00 9.41800000e+02 0.00000000e+00
+  1.53333333e+00 0.00000000e+00]
+ [7.33333333e-01 2.66666667e+00 6.06666667e+00 2.80000000e+00
+  1.73333333e+00 0.00000000e+00 0.00000000e+00 1.00633333e+03
+  2.53333333e+00 5.13333333e+00]
+ [1.93333333e+00 2.00000000e-01 2.60000000e+00 5.26666667e+00
+  6.66666667e-01 2.40000000e+00 1.86666667e+00 2.46666667e+00
+  9.52533333e+02 4.06666667e+00]
+ [1.60000000e+00 2.40000000e+00 4.00000000e-01 3.20000000e+00
+  7.26666667e+00 3.40000000e+00 1.53333333e+00 4.86666667e+00
+  1.73333333e+00 9.82600000e+02]]</t>
+  </si>
+  <si>
+    <t>LBFGS With LS</t>
+  </si>
+  <si>
+    <t>98.08%</t>
   </si>
 </sst>
 </file>
@@ -581,10 +581,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -890,14 +893,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="5" max="5" width="16.7109375" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" customWidth="1"/>
+    <col min="6" max="6" width="128.85546875" customWidth="1"/>
     <col min="7" max="7" width="46.140625" customWidth="1"/>
     <col min="8" max="8" width="25.140625" customWidth="1"/>
   </cols>
@@ -931,44 +934,44 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D2">
+        <v>40290.797656249997</v>
+      </c>
+      <c r="E2">
+        <v>15.133333333333329</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="G2" t="s">
+        <v>54</v>
+      </c>
+      <c r="H2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2">
-        <v>34279.996614583331</v>
-      </c>
-      <c r="E2">
-        <v>9.7333333333333325</v>
-      </c>
-      <c r="F2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" t="s">
-        <v>63</v>
-      </c>
-      <c r="H2" t="s">
-        <v>13</v>
-      </c>
       <c r="I2" t="s">
-        <v>14</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="D3">
         <v>35359.81145833333</v>
@@ -977,27 +980,27 @@
         <v>9.6</v>
       </c>
       <c r="F3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="G3" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="H3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="I3" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="D4">
         <v>33985.24309895833</v>
@@ -1006,27 +1009,27 @@
         <v>9.4</v>
       </c>
       <c r="F4" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="G4" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="H4" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="I4" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D5">
         <v>33900.55963541667</v>
@@ -1035,27 +1038,27 @@
         <v>16.399999999999999</v>
       </c>
       <c r="F5" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="G5" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="H5" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="I5" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C6" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D6">
         <v>33572.33489583333</v>
@@ -1064,56 +1067,56 @@
         <v>14.33333333333333</v>
       </c>
       <c r="F6" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="G6" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="H6" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="I6" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>33</v>
+        <v>67</v>
       </c>
       <c r="B7" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C7" t="s">
-        <v>35</v>
+        <v>68</v>
       </c>
       <c r="D7">
-        <v>10116.9154296875</v>
+        <v>10159.117578125</v>
       </c>
       <c r="E7">
-        <v>2.2000000000000002</v>
+        <v>2.6</v>
       </c>
       <c r="F7" t="s">
-        <v>36</v>
+        <v>69</v>
       </c>
       <c r="G7" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="H7" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="I7" t="s">
-        <v>38</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="B8" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="C8" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="D8">
         <v>6471.6047526041666</v>
@@ -1122,27 +1125,27 @@
         <v>58.93333333333333</v>
       </c>
       <c r="F8" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="G8" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="H8" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="I8" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="B9" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="C9" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="D9">
         <v>32759.5234375</v>
@@ -1151,27 +1154,27 @@
         <v>84.8</v>
       </c>
       <c r="F9" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="G9" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="H9" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="I9" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="B10" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="C10" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="D10">
         <v>47466.754427083331</v>
@@ -1180,27 +1183,27 @@
         <v>13.46666666666667</v>
       </c>
       <c r="F10" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="G10" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="H10" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="I10" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C11" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="D11">
         <v>33021.297526041657</v>
@@ -1209,16 +1212,16 @@
         <v>9.3333333333333339</v>
       </c>
       <c r="F11" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="G11" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="H11" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="I11" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>